<commit_message>
"Added some analysis sections, changed formatting"
</commit_message>
<xml_diff>
--- a/Experiment #4/PreLab_Design.xlsx
+++ b/Experiment #4/PreLab_Design.xlsx
@@ -339,11 +339,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2133038944"/>
-        <c:axId val="-2112461712"/>
+        <c:axId val="2130018336"/>
+        <c:axId val="2130021760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2133038944"/>
+        <c:axId val="2130018336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -386,7 +386,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2112461712"/>
+        <c:crossAx val="2130021760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -394,7 +394,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2112461712"/>
+        <c:axId val="2130021760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -445,7 +445,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2133038944"/>
+        <c:crossAx val="2130018336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1373,8 +1373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
"Eric section's almost finished- need schematic diagrams, state machine annotations, maybe some timing diagrams(?)"
</commit_message>
<xml_diff>
--- a/Experiment #4/PreLab_Design.xlsx
+++ b/Experiment #4/PreLab_Design.xlsx
@@ -48,13 +48,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="PT Serif"/>
     </font>
   </fonts>
   <fills count="2">
@@ -77,8 +82,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -339,11 +345,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2130018336"/>
-        <c:axId val="2130021760"/>
+        <c:axId val="-2073294464"/>
+        <c:axId val="-2074264384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2130018336"/>
+        <c:axId val="-2073294464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -386,7 +392,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2130021760"/>
+        <c:crossAx val="-2074264384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -394,7 +400,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2130021760"/>
+        <c:axId val="-2074264384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -445,7 +451,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2130018336"/>
+        <c:crossAx val="-2073294464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1374,68 +1380,70 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="15" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <f>(156.39/156.65)</f>
         <v>0.9983402489626555</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <f>156.3/156.65</f>
         <v>0.99776571975742101</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <f>64.526/62.81</f>
         <v>1.0273204903677757</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <f>61.55/62.81</f>
         <v>0.97993950007960506</v>
       </c>

</xml_diff>